<commit_message>
added age group SSPM0_4 and SSPF0_4
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/SSP_DRI_ageGroupLookUp.xlsx
+++ b/data-raw/NutrientData/SSP_DRI_ageGroupLookUp.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27217"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutrientModeling/data-raw/NutrientData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t>male.ssp</t>
   </si>
@@ -195,6 +198,12 @@
   </si>
   <si>
     <t>SSPF100Plus</t>
+  </si>
+  <si>
+    <t>SSPM0_4</t>
+  </si>
+  <si>
+    <t>SSPF0_4</t>
   </si>
 </sst>
 </file>
@@ -509,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,13 +542,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -547,55 +556,55 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -603,27 +612,27 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -631,13 +640,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -645,13 +654,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
@@ -659,13 +668,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
@@ -673,27 +682,27 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
@@ -701,13 +710,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
@@ -715,27 +724,27 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>44</v>
@@ -743,13 +752,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
         <v>44</v>
@@ -757,13 +766,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
         <v>44</v>
@@ -771,13 +780,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>44</v>
@@ -785,13 +794,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
         <v>44</v>
@@ -799,15 +808,29 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
         <v>42</v>
       </c>
       <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
         <v>56</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rewrote dataPrep.NutrientRequirements.R to be faster and more transparent. Minor updates to automate.R Add IMPACT regions update June 6 2016.xlsx. Updated the SSP_DRI_ageGroupLookup as part of the nutrequirements rewrite.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/SSP_DRI_ageGroupLookUp.xlsx
+++ b/data-raw/NutrientData/SSP_DRI_ageGroupLookUp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30920" yWindow="-3320" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="-30620" yWindow="-3320" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,19 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
-  <si>
-    <t>male.ssp</t>
-  </si>
-  <si>
-    <t>male.dri</t>
-  </si>
-  <si>
-    <t>female.ssp</t>
-  </si>
-  <si>
-    <t>female.dri</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
   <si>
     <t>SSPM5_9</t>
   </si>
@@ -204,6 +192,30 @@
   </si>
   <si>
     <t>SSPF0_4</t>
+  </si>
+  <si>
+    <t>Chil0_3</t>
+  </si>
+  <si>
+    <t>ssp</t>
+  </si>
+  <si>
+    <t>dri</t>
+  </si>
+  <si>
+    <t>SSPF15_49</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SSPLact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSPPreg </t>
+  </si>
+  <si>
+    <t>LactTot</t>
+  </si>
+  <si>
+    <t>PregTot</t>
   </si>
 </sst>
 </file>
@@ -518,320 +530,380 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" t="s">
-        <v>44</v>
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up various minor bugs
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/SSP_DRI_ageGroupLookUp.xlsx
+++ b/data-raw/NutrientData/SSP_DRI_ageGroupLookUp.xlsx
@@ -206,16 +206,16 @@
     <t>SSPF15_49</t>
   </si>
   <si>
-    <t xml:space="preserve"> SSPLact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSPPreg </t>
-  </si>
-  <si>
     <t>LactTot</t>
   </si>
   <si>
     <t>PregTot</t>
+  </si>
+  <si>
+    <t>SSPLact</t>
+  </si>
+  <si>
+    <t>SSPPreg</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -892,18 +892,18 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
         <v>59</v>
-      </c>
-      <c r="B45" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" t="s">
         <v>60</v>
-      </c>
-      <c r="B46" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>